<commit_message>
added requirements list file
</commit_message>
<xml_diff>
--- a/instance/downloads/timeentrydownload.xlsx
+++ b/instance/downloads/timeentrydownload.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,7 +488,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>erit gridnev</t>
+          <t>Erit Gridnev</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -532,32 +532,32 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-06-04 00:00:00</t>
+          <t>2024-06-08 00:00:00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16:59:46</t>
+          <t>17:23:50</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>17:26:00</t>
+          <t>17:24:17</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>17</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>OREN LAVI</t>
+          <t>Avi Semah</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0:26:14</t>
+          <t>0:00:27</t>
         </is>
       </c>
     </row>
@@ -569,89 +569,57 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>17:23:50</t>
+          <t>17:37:22</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>17:24:17</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>19</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Avi Semah</t>
+          <t>Shir Semah</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0:00:27</t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-06-08 00:00:00</t>
+          <t>2024-06-09 00:00:00</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>17:37:22</t>
+          <t>1:58:00</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>2:58:00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>17</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Shir Semah</t>
+          <t>Avi Semah</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2024-06-09 00:00:00</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>1:58:00</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>2:58:00</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Avi Semah</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
         <is>
           <t>1:00:00</t>
         </is>

</xml_diff>